<commit_message>
Some reorganization input file and datafiles
changes: errorbars, ordening...
</commit_message>
<xml_diff>
--- a/Code/emissions_2014.xlsx
+++ b/Code/emissions_2014.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janbo\OneDrive\Documenten\GitHub\MethylChloroformSOAC\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B0BE8A3-961B-4C2F-9CA2-EDD125304678}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7714C406-1AA9-46A7-9565-993A64CD907B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F383D424-2CEF-4764-971B-13A0AD9DC4F1}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>CH3CCl3 (Gg/yr)</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>CFC-12 (Gg/yr)</t>
+  </si>
+  <si>
+    <t>time</t>
   </si>
 </sst>
 </file>
@@ -401,12 +404,15 @@
   <dimension ref="A1:D64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>